<commit_message>
moved LEDs on bottom side. Created a custome bottom part of enclosure RL6015
</commit_message>
<xml_diff>
--- a/kicad/Design-doc/EISScube v3.0 LTE-BOM-case-connector.xlsx
+++ b/kicad/Design-doc/EISScube v3.0 LTE-BOM-case-connector.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yuriy/Dropbox/EISScube v3.0 LTE/Design-doc/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yuriy/Projects/eisscubeLTEhardware/kicad/Design-doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{68FAB5DA-C622-B64A-A85B-3D0A87001E61}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{672BC806-4ED6-264A-A592-242D00032937}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6420" yWindow="460" windowWidth="43860" windowHeight="26740"/>
+    <workbookView xWindow="4580" yWindow="460" windowWidth="43860" windowHeight="26740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EISScube v3.0 LTE-BOM-case-conn" sheetId="1" r:id="rId1"/>
@@ -127,9 +127,6 @@
     <t xml:space="preserve">C28, </t>
   </si>
   <si>
-    <t>470uF 35V</t>
-  </si>
-  <si>
     <t>Capacitors_SMD:CP_Elec_10x10.5</t>
   </si>
   <si>
@@ -139,9 +136,6 @@
     <t xml:space="preserve">C30, </t>
   </si>
   <si>
-    <t>330uF 16V</t>
-  </si>
-  <si>
     <t xml:space="preserve">C32, C35, </t>
   </si>
   <si>
@@ -589,12 +583,6 @@
     <t>Case</t>
   </si>
   <si>
-    <t>EverestCase-PCO15</t>
-  </si>
-  <si>
-    <t>Clousure case (need to ask for customization - make a opening and hole)</t>
-  </si>
-  <si>
     <t>SMA Jack (edge mount)</t>
   </si>
   <si>
@@ -602,12 +590,24 @@
   </si>
   <si>
     <t>External</t>
+  </si>
+  <si>
+    <t>220uF 35V</t>
+  </si>
+  <si>
+    <t>470uF 16V</t>
+  </si>
+  <si>
+    <t>RITEC Enclosures - RL6015</t>
+  </si>
+  <si>
+    <t>Clousure case (need to ask for customization - make a 4 holes in bottom part)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1459,7 +1459,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -1481,7 +1481,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1539,7 +1539,7 @@
         <v>13</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -1703,69 +1703,69 @@
         <v>1</v>
       </c>
       <c r="C17" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="E17" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B18" s="1">
         <v>1</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>39</v>
+        <v>191</v>
       </c>
       <c r="D18" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E18" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B19" s="1">
         <v>2</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B20" s="1">
         <v>6</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B21" s="1">
         <v>3</v>
@@ -1774,7 +1774,7 @@
         <v>31</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>17</v>
@@ -1782,716 +1782,716 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B22" s="1">
         <v>5</v>
       </c>
       <c r="C22" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E22" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B23" s="1">
         <v>7</v>
       </c>
       <c r="C23" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E23" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B24" s="1">
+        <v>1</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D24" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B24" s="1">
-        <v>1</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>58</v>
-      </c>
       <c r="E24" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B25" s="1">
+        <v>1</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D25" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B25" s="1">
-        <v>1</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>61</v>
-      </c>
       <c r="E25" s="1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B26" s="1">
         <v>3</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B27" s="1">
+        <v>1</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D27" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B27" s="1">
-        <v>1</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>66</v>
-      </c>
       <c r="E27" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B28" s="1">
+        <v>1</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D28" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B28" s="1">
-        <v>1</v>
-      </c>
-      <c r="C28" s="1" t="s">
+      <c r="E28" s="1" t="s">
         <v>68</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B29" s="1">
+        <v>1</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D29" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B29" s="1">
-        <v>1</v>
-      </c>
-      <c r="C29" s="1" t="s">
+      <c r="E29" s="1" t="s">
         <v>72</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B30" s="1">
+        <v>1</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D30" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B30" s="1">
-        <v>1</v>
-      </c>
-      <c r="C30" s="1" t="s">
+      <c r="E30" s="1" t="s">
         <v>76</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B31" s="1">
+        <v>1</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D31" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B31" s="1">
-        <v>1</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>81</v>
-      </c>
       <c r="E31" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B32" s="1">
+        <v>1</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D32" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B32" s="1">
-        <v>1</v>
-      </c>
-      <c r="C32" s="1" t="s">
+      <c r="E32" s="1" t="s">
         <v>83</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B33" s="1">
+        <v>1</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D33" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B33" s="1">
-        <v>1</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>88</v>
-      </c>
       <c r="E33" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B34" s="1">
+        <v>1</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D34" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B34" s="1">
-        <v>1</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>91</v>
-      </c>
       <c r="E34" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B35" s="1">
+        <v>1</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D35" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B35" s="1">
-        <v>1</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>94</v>
-      </c>
       <c r="E35" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B36" s="1">
         <v>1</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B37" s="1">
+        <v>1</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D37" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B37" s="1">
-        <v>1</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>99</v>
-      </c>
       <c r="E37" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B38" s="1">
         <v>4</v>
       </c>
       <c r="C38" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E38" s="1" t="s">
         <v>101</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B39" s="1">
+        <v>1</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D39" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="B39" s="1">
-        <v>1</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>106</v>
-      </c>
       <c r="E39" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B40" s="1">
+        <v>1</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D40" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B40" s="1">
-        <v>1</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>109</v>
-      </c>
       <c r="E40" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B41" s="1">
         <v>1</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B42" s="1">
         <v>1</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B43" s="1">
         <v>13</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B44" s="1">
         <v>3</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B45" s="1">
         <v>1</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B46" s="1">
         <v>7</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B47" s="1">
         <v>1</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B48" s="1">
         <v>1</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B49" s="1">
+        <v>1</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D49" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="B49" s="1">
-        <v>1</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>127</v>
-      </c>
       <c r="E49" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B50" s="1">
         <v>8</v>
       </c>
       <c r="C50" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="E50" s="1" t="s">
         <v>129</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="E50" s="1" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B51" s="1">
+        <v>1</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D51" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="B51" s="1">
-        <v>1</v>
-      </c>
-      <c r="C51" s="1" t="s">
+      <c r="E51" s="1" t="s">
         <v>133</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="E51" s="1" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B52" s="1">
+        <v>1</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D52" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="B52" s="1">
-        <v>1</v>
-      </c>
-      <c r="C52" s="1" t="s">
+      <c r="E52" s="1" t="s">
         <v>137</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="E52" s="1" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B53" s="1">
+        <v>1</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="D53" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="B53" s="1">
-        <v>1</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>142</v>
-      </c>
       <c r="E53" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B54" s="1">
+        <v>1</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="D54" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="B54" s="1">
-        <v>1</v>
-      </c>
-      <c r="C54" s="1" t="s">
+      <c r="E54" s="1" t="s">
         <v>144</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="E54" s="1" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B55" s="1">
+        <v>1</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="D55" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="B55" s="1">
-        <v>1</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="D55" s="1" t="s">
-        <v>149</v>
-      </c>
       <c r="E55" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B56" s="1">
+        <v>1</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="D56" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="B56" s="1">
-        <v>1</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="D56" s="1" t="s">
-        <v>152</v>
-      </c>
       <c r="E56" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="B57" s="1">
+        <v>1</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="D57" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="B57" s="1">
-        <v>1</v>
-      </c>
-      <c r="C57" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="D57" s="1" t="s">
-        <v>155</v>
-      </c>
       <c r="E57" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B58" s="1">
         <v>1</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="B59" s="1">
+        <v>1</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="D59" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="B59" s="1">
-        <v>1</v>
-      </c>
-      <c r="C59" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="D59" s="1" t="s">
-        <v>160</v>
-      </c>
       <c r="E59" s="1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="B60" s="1">
+        <v>1</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="D60" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="B60" s="1">
-        <v>1</v>
-      </c>
-      <c r="C60" s="1" t="s">
+      <c r="E60" s="1" t="s">
         <v>162</v>
-      </c>
-      <c r="D60" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="E60" s="1" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B61" s="1">
+        <v>1</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="D61" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="B61" s="1">
-        <v>1</v>
-      </c>
-      <c r="C61" s="1" t="s">
+      <c r="E61" s="1" t="s">
         <v>166</v>
-      </c>
-      <c r="D61" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="E61" s="1" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B62" s="1">
         <v>1</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="B63" s="1">
+        <v>1</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="E63" s="1" t="s">
         <v>193</v>
-      </c>
-      <c r="B63" s="1">
-        <v>1</v>
-      </c>
-      <c r="C63" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="D63" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="E63" s="1" t="s">
-        <v>190</v>
       </c>
     </row>
   </sheetData>

</xml_diff>